<commit_message>
Author name: Shitij Khanna
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/ShitijKhanna.xlsx
+++ b/TeamDetails/TasksBreakDown/ShitijKhanna.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shitij khanna.admin-PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\internsdhip\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>story ID</t>
   </si>
@@ -103,38 +103,17 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> T_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      T_1</t>
-  </si>
-  <si>
-    <t>T-3</t>
-  </si>
-  <si>
     <t>Make block diagram of the entire code journey.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> T_4</t>
   </si>
   <si>
     <t xml:space="preserve">      Technical Understanding of the story.
 Which languages (Angular,Bootstarp) is used to implement the story .    </t>
   </si>
   <si>
-    <t>T_5</t>
-  </si>
-  <si>
     <t>Unit Testing</t>
   </si>
   <si>
-    <t xml:space="preserve">  T_6</t>
-  </si>
-  <si>
     <t>Code Review</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> T_7</t>
   </si>
   <si>
     <t>Incorporate code review comments.</t>
@@ -162,18 +141,6 @@
     <t>Understanding forward and backward linkages.</t>
   </si>
   <si>
-    <t>T_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> T_5</t>
-  </si>
-  <si>
-    <t>T_6</t>
-  </si>
-  <si>
-    <t>T_7</t>
-  </si>
-  <si>
     <t>4 hrs</t>
   </si>
   <si>
@@ -184,9 +151,6 @@
   </si>
   <si>
     <t xml:space="preserve">           2 hrs</t>
-  </si>
-  <si>
-    <t>T_4</t>
   </si>
   <si>
     <t>24 hrs</t>
@@ -197,6 +161,39 @@
   <si>
     <t xml:space="preserve">      Technical Understanding of the story.
 Which languages (HTML) is used to implement the story .    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      T-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T-02</t>
+  </si>
+  <si>
+    <t>T-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T-04</t>
+  </si>
+  <si>
+    <t>T-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  T-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T-07</t>
+  </si>
+  <si>
+    <t>T-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T-05</t>
+  </si>
+  <si>
+    <t>T-06</t>
+  </si>
+  <si>
+    <t>T-07</t>
   </si>
 </sst>
 </file>
@@ -234,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -325,16 +322,181 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -342,17 +504,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,19 +544,68 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,329 +904,338 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+    </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="29"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="30"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="31"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="31"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="29"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="32"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="30"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="31"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="32"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="32"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="17" t="s">
+      <c r="C16" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="17" t="s">
+      <c r="F16" s="26"/>
+      <c r="G16" s="27"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="29"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="32"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="28"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="17" t="s">
+      <c r="E19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="32"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="5" t="s">
+      <c r="F20" s="9"/>
+      <c r="G20" s="30"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="31"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="29"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="32"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="28"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="17" t="s">
+      <c r="E24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="32"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="33"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="7" t="s">
+      <c r="E25" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="37"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="A26" s="2"/>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Author Name :   Shitij Khanna
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/ShitijKhanna.xlsx
+++ b/TeamDetails/TasksBreakDown/ShitijKhanna.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t>story ID</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 2 hrs</t>
+  </si>
+  <si>
+    <t>Populate the table in the BA page below the search option.</t>
+  </si>
+  <si>
+    <t>6 hrs.</t>
   </si>
 </sst>
 </file>
@@ -526,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -576,12 +582,78 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -597,21 +669,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -629,57 +692,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,93 +1013,93 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="19" t="s">
+      <c r="F3" s="32"/>
+      <c r="G3" s="28" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="20"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="20" t="s">
+      <c r="A5" s="41"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="47"/>
-      <c r="G5" s="20" t="s">
+      <c r="F5" s="34"/>
+      <c r="G5" s="29" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="20"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="20"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="20"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="29"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1103,43 +1115,43 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="20" t="s">
+      <c r="A10" s="41"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="50"/>
-      <c r="G10" s="20" t="s">
+      <c r="F10" s="37"/>
+      <c r="G10" s="29" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="20"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="20"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="29"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="22"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="7" t="s">
         <v>29</v>
       </c>
@@ -1155,8 +1167,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="7" t="s">
         <v>30</v>
       </c>
@@ -1172,8 +1184,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="29"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="11" t="s">
         <v>31</v>
       </c>
@@ -1189,51 +1201,51 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="41"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="20"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="29"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="20"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="6" t="s">
         <v>26</v>
       </c>
@@ -1251,8 +1263,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="20"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="6" t="s">
         <v>27</v>
       </c>
@@ -1270,63 +1282,63 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20" t="s">
+      <c r="A21" s="41"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="51" t="s">
+      <c r="D21" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>63</v>
+      <c r="F21" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="29">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="20"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="29"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="20"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="29"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="20"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="29"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="20"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="29"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="20"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="10" t="s">
         <v>29</v>
       </c>
@@ -1344,47 +1356,47 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="10" t="s">
+      <c r="A27" s="41"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="41"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D28" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>53</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>54</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="20"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="10" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>54</v>
@@ -1395,30 +1407,30 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" s="20"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
-      <c r="B31" s="20"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>53</v>
@@ -1429,118 +1441,119 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="20"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="41"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="10" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>54</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="41"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="6" t="s">
+      <c r="F34" s="9"/>
+      <c r="G34" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="41"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="41"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="27"/>
-      <c r="B36" s="52"/>
-      <c r="C36" s="13" t="s">
+      <c r="F36" s="3"/>
+      <c r="G36" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="42"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D37" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E37" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="14" t="s">
+      <c r="F37" s="12"/>
+      <c r="G37" s="14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="C37" s="1"/>
-    </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C39" s="1"/>
     </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="F21:F25"/>
-    <mergeCell ref="G21:G25"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F8"/>
-    <mergeCell ref="G5:G8"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="B17:B36"/>
-    <mergeCell ref="A17:A36"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="E21:E25"/>
     <mergeCell ref="C17:C18"/>
@@ -1556,6 +1569,22 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D5:D8"/>
     <mergeCell ref="C5:C8"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="F21:F25"/>
+    <mergeCell ref="G21:G25"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F8"/>
+    <mergeCell ref="G5:G8"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="B17:B37"/>
+    <mergeCell ref="A17:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author Name : Shitij Khanna File Added  : ShitijKhanna.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/ShitijKhanna.xlsx
+++ b/TeamDetails/TasksBreakDown/ShitijKhanna.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
   <si>
     <t>story ID</t>
   </si>
@@ -227,13 +227,19 @@
     <t>DONE</t>
   </si>
   <si>
-    <t xml:space="preserve">  IN dev</t>
-  </si>
-  <si>
     <t>SSDMS-57</t>
   </si>
   <si>
     <t xml:space="preserve">   DONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  DONE</t>
+  </si>
+  <si>
+    <t>IN DEV</t>
+  </si>
+  <si>
+    <t>IN PROG</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -550,7 +556,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,10 +609,104 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -630,91 +729,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,621 +1052,671 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="51">
         <v>22</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="51">
         <v>3</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="30">
+      <c r="F3" s="46">
         <v>3</v>
       </c>
-      <c r="H3" s="65"/>
+      <c r="G3" s="51">
+        <v>0</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="65"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30" t="s">
+      <c r="A5" s="51"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="51">
         <v>6</v>
       </c>
-      <c r="F5" s="59"/>
-      <c r="G5" s="30">
+      <c r="F5" s="48">
         <v>6</v>
       </c>
-      <c r="H5" s="65"/>
+      <c r="G5" s="51">
+        <v>0</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="65"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="65"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="36"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="65"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="36"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="14" t="s">
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="15">
         <v>2</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="16">
+      <c r="F9" s="28">
         <v>2</v>
       </c>
-      <c r="H9" s="28"/>
+      <c r="G9" s="15">
+        <v>0</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30" t="s">
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="51">
         <v>6</v>
       </c>
-      <c r="F10" s="57"/>
-      <c r="G10" s="30">
+      <c r="F10" s="46"/>
+      <c r="G10" s="51">
         <v>6</v>
       </c>
-      <c r="H10" s="65"/>
+      <c r="H10" s="36" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="65"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="36"/>
     </row>
     <row r="12" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="65"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="36"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="16" t="s">
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="15">
         <v>3</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="16">
+      <c r="F13" s="16"/>
+      <c r="G13" s="15">
         <v>3</v>
       </c>
-      <c r="H13" s="28"/>
+      <c r="H13" s="29"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="16" t="s">
+      <c r="A14" s="51"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="15">
         <v>1</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="16">
+      <c r="F14" s="16"/>
+      <c r="G14" s="15">
         <v>1</v>
       </c>
-      <c r="H14" s="28"/>
+      <c r="H14" s="29"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="16" t="s">
+      <c r="A15" s="51"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="15">
         <v>1</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="16">
+      <c r="F15" s="16"/>
+      <c r="G15" s="15">
         <v>1</v>
       </c>
-      <c r="H15" s="28"/>
+      <c r="H15" s="29"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="11">
+      <c r="E16" s="5">
         <v>22</v>
       </c>
-      <c r="H16" s="29"/>
+      <c r="F16" s="5">
+        <v>11</v>
+      </c>
+      <c r="G16" s="10">
+        <v>11</v>
+      </c>
+      <c r="H16" s="30"/>
     </row>
     <row r="17" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="18"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="45">
+        <v>43</v>
+      </c>
+      <c r="C18" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="45">
+        <v>4</v>
+      </c>
+      <c r="F18" s="44">
+        <v>4</v>
+      </c>
+      <c r="G18" s="45">
+        <v>0</v>
+      </c>
+      <c r="H18" s="37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="56"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="56"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="21">
+        <v>6</v>
+      </c>
+      <c r="F20" s="19">
+        <v>6</v>
+      </c>
+      <c r="G20" s="21">
+        <v>0</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="56"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="21">
+        <v>2</v>
+      </c>
+      <c r="F21" s="19">
+        <v>2</v>
+      </c>
+      <c r="G21" s="21">
+        <v>0</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" s="38"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="56"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="37">
+        <v>6</v>
+      </c>
+      <c r="F22" s="32">
+        <v>6</v>
+      </c>
+      <c r="G22" s="37">
+        <v>0</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" s="38"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="56"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="38"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="56"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="38"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="56"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="38"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="56"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="38"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="56"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="18">
+        <v>1</v>
+      </c>
+      <c r="F27" s="22">
+        <v>1</v>
+      </c>
+      <c r="G27" s="18">
+        <v>0</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="56"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="18">
+        <v>3</v>
+      </c>
+      <c r="F28" s="22">
+        <v>3</v>
+      </c>
+      <c r="G28" s="18">
+        <v>0</v>
+      </c>
+      <c r="H28" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="41">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="56"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="18">
+        <v>2</v>
+      </c>
+      <c r="F29" s="22">
+        <v>2</v>
+      </c>
+      <c r="G29" s="18">
+        <v>0</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="56"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="18">
+        <v>3</v>
+      </c>
+      <c r="F30" s="22">
+        <v>3</v>
+      </c>
+      <c r="G30" s="18">
+        <v>0</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="56"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="18">
+        <v>3</v>
+      </c>
+      <c r="F31" s="22">
+        <v>3</v>
+      </c>
+      <c r="G31" s="18">
+        <v>0</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="56"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="41">
-        <v>4</v>
-      </c>
-      <c r="F18" s="53">
-        <v>4</v>
-      </c>
-      <c r="G18" s="41">
+      <c r="D32" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="18">
+        <v>2</v>
+      </c>
+      <c r="F32" s="22">
+        <v>2</v>
+      </c>
+      <c r="G32" s="18">
         <v>0</v>
       </c>
-      <c r="H18" s="42" t="s">
+      <c r="H32" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="22">
-        <v>6</v>
-      </c>
-      <c r="F20" s="20">
-        <v>6</v>
-      </c>
-      <c r="G20" s="22">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="56"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="18">
+        <v>2</v>
+      </c>
+      <c r="F33" s="22">
+        <v>2</v>
+      </c>
+      <c r="G33" s="18">
         <v>0</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H33" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="22">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="56"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="18">
+        <v>1</v>
+      </c>
+      <c r="F34" s="22">
+        <v>1</v>
+      </c>
+      <c r="G34" s="18">
+        <v>0</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="56"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="18">
+        <v>3</v>
+      </c>
+      <c r="F35" s="22">
+        <v>3</v>
+      </c>
+      <c r="G35" s="18">
+        <v>0</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="56"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="21">
         <v>2</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F36" s="19">
         <v>2</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G36" s="21">
         <v>0</v>
       </c>
-      <c r="H21" s="22" t="s">
+      <c r="H36" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="I21" s="47"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="63" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="42">
-        <v>6</v>
-      </c>
-      <c r="F22" s="55">
-        <v>6</v>
-      </c>
-      <c r="G22" s="42">
-        <v>0</v>
-      </c>
-      <c r="H22" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22" s="47"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="47"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="47"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="47"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="47"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="19">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="56"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="21">
         <v>1</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F37" s="19"/>
+      <c r="G37" s="21">
         <v>1</v>
       </c>
-      <c r="G27" s="19">
-        <v>0</v>
-      </c>
-      <c r="H27" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="39"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="19">
-        <v>3</v>
-      </c>
-      <c r="F28" s="23">
-        <v>3</v>
-      </c>
-      <c r="G28" s="19">
-        <v>0</v>
-      </c>
-      <c r="H28" s="66" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="39"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="19">
+      <c r="H37" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="57"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="25">
         <v>2</v>
       </c>
-      <c r="F29" s="23"/>
-      <c r="G29" s="19">
+      <c r="F38" s="26"/>
+      <c r="G38" s="25">
         <v>2</v>
       </c>
-      <c r="H29" s="66" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="39"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="19">
-        <v>3</v>
-      </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="19">
-        <v>3</v>
-      </c>
-      <c r="H30" s="21"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="39"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="19">
-        <v>3</v>
-      </c>
-      <c r="F31" s="23"/>
-      <c r="G31" s="19">
-        <v>3</v>
-      </c>
-      <c r="H31" s="21"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="39"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" s="19">
-        <v>2</v>
-      </c>
-      <c r="F32" s="23"/>
-      <c r="G32" s="19">
-        <v>2</v>
-      </c>
-      <c r="H32" s="21"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="19">
-        <v>2</v>
-      </c>
-      <c r="F33" s="23"/>
-      <c r="G33" s="19">
-        <v>2</v>
-      </c>
-      <c r="H33" s="21"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="39"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="19">
-        <v>1</v>
-      </c>
-      <c r="F34" s="23"/>
-      <c r="G34" s="19">
-        <v>1</v>
-      </c>
-      <c r="H34" s="21"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="39"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="19">
-        <v>3</v>
-      </c>
-      <c r="F35" s="23"/>
-      <c r="G35" s="19">
-        <v>3</v>
-      </c>
-      <c r="H35" s="21"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="39"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="22">
-        <v>2</v>
-      </c>
-      <c r="F36" s="21"/>
-      <c r="G36" s="22">
-        <v>2</v>
-      </c>
-      <c r="H36" s="21"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="39"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="22">
-        <v>1</v>
-      </c>
-      <c r="F37" s="21"/>
-      <c r="G37" s="22">
-        <v>1</v>
-      </c>
-      <c r="H37" s="21"/>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="40"/>
-      <c r="B38" s="64"/>
-      <c r="C38" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="26">
-        <v>2</v>
-      </c>
-      <c r="F38" s="27"/>
-      <c r="G38" s="26">
-        <v>2</v>
-      </c>
-      <c r="H38" s="21"/>
+      <c r="H38" s="20"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="7">
         <f>SUM(E18:E38)</f>
         <v>43</v>
       </c>
-      <c r="F39" s="8">
-        <v>22</v>
-      </c>
-      <c r="G39" s="8">
+      <c r="F39" s="7">
+        <v>40</v>
+      </c>
+      <c r="G39" s="7">
         <f>SUM(G18:G38)</f>
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1660,14 +1724,29 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="1"/>
+      <c r="G41">
+        <f>SUM(G39,G16)</f>
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="H22:H26"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="H5:H8"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="A3:A15"/>
+    <mergeCell ref="B3:B15"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="A18:A38"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
     <mergeCell ref="I21:I26"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A17:G17"/>
@@ -1684,22 +1763,11 @@
     <mergeCell ref="D22:D26"/>
     <mergeCell ref="C22:C26"/>
     <mergeCell ref="B18:B38"/>
-    <mergeCell ref="A18:A38"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="A3:A15"/>
-    <mergeCell ref="B3:B15"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="H22:H26"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H5:H8"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="H18:H19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>